<commit_message>
Finished excel sheet for expansion spoils
</commit_message>
<xml_diff>
--- a/Random/Cards/SpoilsCardActions.xlsx
+++ b/Random/Cards/SpoilsCardActions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>#Uses</t>
   </si>
@@ -107,15 +107,6 @@
     <t>Lucky Day</t>
   </si>
   <si>
-    <t>Can Start With?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +6 spoils cards</t>
   </si>
   <si>
@@ -140,13 +131,106 @@
     <t>After successful Encounter/Mission</t>
   </si>
   <si>
-    <t>EVENT</t>
-  </si>
-  <si>
     <t>5.56mm Light Machinegun</t>
   </si>
   <si>
     <t xml:space="preserve"> +1 prestige</t>
+  </si>
+  <si>
+    <t>9mm Semi Automatic Pistol</t>
+  </si>
+  <si>
+    <t>Five 9MM Semi Auto Pistols</t>
+  </si>
+  <si>
+    <t>Armored Car</t>
+  </si>
+  <si>
+    <t>Discard Ambush encounters for another from the same deck</t>
+  </si>
+  <si>
+    <t>After drawing Ambush encounter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +2 movement</t>
+  </si>
+  <si>
+    <t>7.62mm Machine Gun</t>
+  </si>
+  <si>
+    <t>Kick Ass Sound System</t>
+  </si>
+  <si>
+    <t>Can't have vehicle = bicycles or horses</t>
+  </si>
+  <si>
+    <t>Jamison Bond's 77 Lotus</t>
+  </si>
+  <si>
+    <t>4d6 damage to opponent OR 2d6 town health removal</t>
+  </si>
+  <si>
+    <t>During PvP OR If within 1 hex of player's town</t>
+  </si>
+  <si>
+    <t>Once OR Once</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +3 movment</t>
+  </si>
+  <si>
+    <t>Pristine American Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +2 salvage</t>
+  </si>
+  <si>
+    <t>End Turn Phase</t>
+  </si>
+  <si>
+    <t>Once per turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +2 prestige</t>
+  </si>
+  <si>
+    <t>Forged Government Credentials</t>
+  </si>
+  <si>
+    <t>Gargantuan BBQ Grill</t>
+  </si>
+  <si>
+    <t>Restrictions</t>
+  </si>
+  <si>
+    <t>4 wheeled vehicle</t>
+  </si>
+  <si>
+    <t>Discard Perishable encounters for another from the same deck</t>
+  </si>
+  <si>
+    <t>After drawing Perishable encounter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -1 Movement</t>
+  </si>
+  <si>
+    <t>Bonus text</t>
+  </si>
+  <si>
+    <t>With 7.62mm M60A3 Turret</t>
+  </si>
+  <si>
+    <t>Compound Hunting Bow</t>
+  </si>
+  <si>
+    <t>With Cooler</t>
+  </si>
+  <si>
+    <t>9mm Auto Pistol</t>
+  </si>
+  <si>
+    <t>Can't start game with (All event cards I think)</t>
   </si>
 </sst>
 </file>
@@ -498,20 +582,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F8E859-266C-4D8A-8E55-872782D0B686}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="66.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -519,79 +604,73 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
+      <c r="G1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -599,7 +678,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -608,10 +687,10 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -619,50 +698,44 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -671,18 +744,15 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -694,47 +764,220 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
-        <v>28</v>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>